<commit_message>
Fixed Titles in Frontispieces to read 'Duke-Edinburgh Edition, Frontispiece, Volume <#>'
</commit_message>
<xml_diff>
--- a/clo-angular/src/assets/albums/fullsize/album_00/Volume0.xlsx
+++ b/clo-angular/src/assets/albums/fullsize/album_00/Volume0.xlsx
@@ -55,7 +55,7 @@
     <t>Publisher</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 1</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 1</t>
   </si>
   <si>
     <t xml:space="preserve">Couriers came to the Grass Market from all over Scotland, and the young Carlyle frequently went there to receive or send boxes and letters from or to Ecclefechan. The Grass Market has changed very little from the early nineteenth century to the present day. </t>
@@ -82,7 +82,7 @@
     <t>Victorian Lives and Letters Consortium</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 2</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 2</t>
   </si>
   <si>
     <t xml:space="preserve">An early portrait of Jane Baillie Welsh made at Haddington by an unknown artist. </t>
@@ -100,7 +100,7 @@
     <t>From the copy in D. A. Wilson, Carlyle, opposite p. 220. The original portrait, which was hanging in Carlyle's house when he died, was handed down in the family of Mrs. Andrew Chrystal, born Jeannie Welsh, Jane's cousin. Francis Jeffrey had the portrait in his possession for some months in 1831, and the Carlyles had difficulty in getting it back from him.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 3</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 3</t>
   </si>
   <si>
     <t xml:space="preserve">Three miniatures of Mrs. Charles Buller, Sr., and her sons Charles and Arthur. </t>
@@ -124,7 +124,7 @@
     <t>From the miniatures in the possession of Harry Grylls, Esq., and used by courtesy of the owner and Lady Mander.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 4</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 4</t>
   </si>
   <si>
     <t>Five caricatures of Edward Irving (ca. 1823). Used as the frontispiece of the Trial of Edward Irving, M.A.: A Cento of Criticism (London: E. Brain, 1823).</t>
@@ -139,7 +139,7 @@
     <t>Volume 4 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 5</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 5</t>
   </si>
   <si>
     <t xml:space="preserve">Copy of an engraving of the Carlyles' home at Craigenputtoch. </t>
@@ -154,7 +154,7 @@
     <t>From an engraving preserved at the Arched House, Ecclefechan.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 6</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 6</t>
   </si>
   <si>
     <t>Silhouettes of Carlyle's father and mother made by Jane Welsh Carlyle with captions in Carlyle's hand, and of Carlyle himself made by Robert Blake from two profile photographs taken in the years shortly before he grew his beard in 1854. The silhouettes of the father and the mother are reproduced from the volume I frontispiece of J. A. Froude, ed., Reminiscences by Thomas Carlyle (London, 1881).</t>
@@ -184,7 +184,7 @@
     <t>The silhouettes of the father and the mother are reproduced from the volume I frontispiece of J. A. Froude, ed., Reminiscences by Thomas Carlyle (London, 1881).</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 7</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 7</t>
   </si>
   <si>
     <t>Photograph of Scotsbrig, near Ecclefechan, home of Carlyle's father and mother from 1826 until their deaths in 1832 and 1853 respectively, and of his youngest brother, James, and his family from 1826 until his death in 1890. Photograph by J. Patrick, courtesy of the University of Edinburgh.</t>
@@ -202,7 +202,7 @@
     <t>Photograph by J. Patrick, courtesy of the University of Edinburgh.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 8</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 8</t>
   </si>
   <si>
     <t>Crayon portrait of Thomas Carlyle by Samuel Laurence, circa 1838. Bought from the artist by John Sterling and greatly admired by him. The original is now at the Carlyle House, Chelsea.</t>
@@ -223,7 +223,7 @@
     <t>The original portrait is now at the Carlyle House, Chelsea.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 9</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 9</t>
   </si>
   <si>
     <t>Chalk portrait of Jane Welsh Carlyle by Samuel Laurence, circa 1838 [1849]. From the original at the Carlyle House, Chelsea.</t>
@@ -235,7 +235,7 @@
     <t>Volume 9 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 10</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 10</t>
   </si>
   <si>
     <t>Oil portrait of Thomas Carlyle by Samuel Laurence, 1838. The original is privately owned; reproduced by kind permission of the owner.</t>
@@ -250,7 +250,7 @@
     <t>The original is privately owned; reproduced by kind permission of the owner.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 11</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 11</t>
   </si>
   <si>
     <t>Lithograph by R. J. Lane, after a drawing by Count Alfred D'Orsay, 1839. The lithograph is reproduced from the copy in the National Portrait Gallery, London. The whereabouts of the original drawing is unknown.</t>
@@ -271,7 +271,7 @@
     <t>The lithograph is reproduced from the copy in the National Portrait Gallery, London. The whereabouts of the original drawing is unknown</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 12</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 12</t>
   </si>
   <si>
     <t>Two photographs; above: Scotsbrig, home of Carlyle's brother James and their mother, ca. 1890, below: Cheyne Row, with bystanders outside number five, ca. 1890. Photographs by J. Patrick, reproduced by permission of the Edinburgh Carlyle Society.</t>
@@ -286,7 +286,7 @@
     <t>Photographs by J. Patrick, reproduced by permission of the Edinburgh Carlyle Society.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 13</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 13</t>
   </si>
   <si>
     <t>Detail of a portrait of Margaret A. Carlyle painted by Maxwell of Dumfries, 1842, Carlyle's House, Chelsea. Reproduced by permission of The National Trust for Places of Historic Interest or Natural Beauty, London.</t>
@@ -307,7 +307,7 @@
     <t>Reproduced by permission of The National Trust for Places of Historic Interest or Natural Beauty, London.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 14</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 14</t>
   </si>
   <si>
     <t>Map of the Thornhill district, Dumfriesshire.</t>
@@ -316,7 +316,7 @@
     <t>Volume 14 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 15</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 15</t>
   </si>
   <si>
     <t>Naseby battlefield and environs.</t>
@@ -325,7 +325,7 @@
     <t>Volume 15 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 16</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 16</t>
   </si>
   <si>
     <t>Oil portrait of Thomas Carlyle by John Linnell, 1843. Courtesy of the National Gallery of Scotland.</t>
@@ -340,7 +340,7 @@
     <t>Courtesy of the National Gallery of Scotland.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 17</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 17</t>
   </si>
   <si>
     <t>Oil portrait of Jane Welsh Carlyle by Spiridione Gambardella, 1843. Privately owned.</t>
@@ -355,7 +355,7 @@
     <t>Original is privately owned.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 18</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 18</t>
   </si>
   <si>
     <t>Oil portrait of Jeannie Welsh (later Chrystal) by Spiridione Gambardella, 1843. Privately owned.</t>
@@ -367,7 +367,7 @@
     <t>Volume 18 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 19</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 19</t>
   </si>
   <si>
     <t>Oil portrait of John Welsh of Liverpool by Spiridione Gambardella, 1854 [1843]. Privately owned.</t>
@@ -379,7 +379,7 @@
     <t>Volume 19 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 20</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 20</t>
   </si>
   <si>
     <t>Daguerreotype of Thomas Carlyle, April 1846, mailed to Ralph Waldo Emerson, 30 April 1846. Reproduced by permission of the Ralph Waldo Emerson Memorial Association and the Houghton Library, Harvard University.</t>
@@ -394,7 +394,7 @@
     <t>Reproduced by permission of the Ralph Waldo Emerson Memorial Association and the Houghton Library, Harvard University.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 21</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 21</t>
   </si>
   <si>
     <t xml:space="preserve">Oil portrait of Lady Harriet Baring by H. W. Pickersgill, R.A. </t>
@@ -412,7 +412,7 @@
     <t>Present whereabouts of original unknown.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 22</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 22</t>
   </si>
   <si>
     <t>Lithograph of Giuseppe Mazzini in the 1840s. Courtesy of the National Portrait Gallery, London.</t>
@@ -430,7 +430,7 @@
     <t>Courtesy of the National Portrait Gallery, London.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 23</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 23</t>
   </si>
   <si>
     <t>Daguerreotype of Ralph Waldo Emerson, London, 1848. By permission of the Houghton Library, Harvard University, bMS Am 1280.235 (706.3A).</t>
@@ -448,7 +448,7 @@
     <t>By permission of the Houghton Library, Harvard University, bMS Am 1280.235 (706.3A).</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 24</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 24</t>
   </si>
   <si>
     <t>Photograph of Thomas Carlyle, 1849 [after 1854]. Reproduced from Sir Charles Gavan Duffy, Conversations with Carlyle (1896).</t>
@@ -460,7 +460,7 @@
     <t>Reproduced from Sir Charles Gavan Duffy, Conversations with Carlyle (1896).</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 25</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 25</t>
   </si>
   <si>
     <t>Jane Welsh Carlyle engraved by J. J. Waddington, Ltd., from an original in water colors and crayon by Carl Hartmann in 1849. Reproduced from Mrs. Brookfield and Her Circle.</t>
@@ -481,7 +481,7 @@
     <t>Reproduced from Mrs. Brookfield and Her Circle.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 26</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 26</t>
   </si>
   <si>
     <t>Medallion of Thomas Carlyle by Thomas Woolner, 1850. Courtesy of the National Galleries of Scotland.</t>
@@ -502,7 +502,7 @@
     <t>Courtesy of the National Galleries of Scotland.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 27</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 27</t>
   </si>
   <si>
     <t>Photograph of Thomas Carlyle by Robert Scott Tait, 31 July 1854. Courtesy of Columbia University Library.</t>
@@ -517,7 +517,7 @@
     <t>Courtesy of Columbia University Library.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 28</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 28</t>
   </si>
   <si>
     <t>Jane Carlyle with the family dog Nero, photographed by Robert Scott Tait, ca. 1853. Courtesy of the National Portrait Gallery, London.</t>
@@ -526,7 +526,7 @@
     <t>Volume 28 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 29</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 29</t>
   </si>
   <si>
     <t>Jane Welsh Carlyle and Geraldine Jewsbury by Robert Scott Tait, April 1855. Courtesy of Columbia University and Edinburgh University Libraries.</t>
@@ -541,7 +541,7 @@
     <t>Courtesy of Columbia University and Edinburgh University Libraries.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 30</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 30</t>
   </si>
   <si>
     <t>Photograph of The Grange, Hampshire, 1972. Reproduced by permission of English Heritage. NMR.</t>
@@ -553,7 +553,7 @@
     <t>Reproduced by permission of English Heritage. NMR.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 31</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 31</t>
   </si>
   <si>
     <t>Jane Welsh Carlyle in the downstairs drawing room, 5 Cheyne Row. Watercolor by Frank Jewsbury, 1856. Privately owned; see also Carlyle Newsletter 7 (Spring 1986): 2.</t>
@@ -571,7 +571,7 @@
     <t>Privately owned; see also Carlyle Newsletter 7 (Spring 1986): 2.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 32</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 32</t>
   </si>
   <si>
     <t>Thomas Carlyle in the attic, 5 Cheyne Row, by Robert Scott Tait, 27 July 1857. Courtesy of Edinburgh University Library.</t>
@@ -583,7 +583,7 @@
     <t>Courtesy of Edinburgh University Library.</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 33</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 33</t>
   </si>
   <si>
     <t>Thomas Carlyle and the family dog Nero at the back door, 5 Cheyne Row, by Robert Scott Tait, 29 July 1857 Courtesy of Edinburgh University Library</t>
@@ -592,7 +592,7 @@
     <t>Volume 33 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 34</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 34</t>
   </si>
   <si>
     <t xml:space="preserve">Map of Dumfries </t>
@@ -601,7 +601,7 @@
     <t>Volume 34 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 35</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 35</t>
   </si>
   <si>
     <t>Sharp, Greenwood, and Fowler, Map of Fife, 1828 (detail) Courtesy of the National Library of Scotland</t>
@@ -616,7 +616,7 @@
     <t>Courtesy of the National Library of Scotland</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 36</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 36</t>
   </si>
   <si>
     <t>"Thomas Carlyle on a midnight ramble"; by Charles Bell Birch, 1859 Courtesy of the National Portrait Gallery</t>
@@ -634,7 +634,7 @@
     <t>Courtesy of the National Portrait Gallery</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 37</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 37</t>
   </si>
   <si>
     <t>Letter from Jane Welsh Carlyle to Mary Baring, 31 January 1861 Courtesy of the National Library of Scotland</t>
@@ -646,7 +646,7 @@
     <t>Volume 37 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 38</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 38</t>
   </si>
   <si>
     <t>Photograph of Thomas Carlyle, by William Jeffrey, September 1862 Courtesy of The National Trust</t>
@@ -661,7 +661,7 @@
     <t>Courtesy of The National Trust</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 39</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 39</t>
   </si>
   <si>
     <t>Photograph of Auchtertool Manse, 1863 Courtesy of Rare Book and Manuscript Library, Columbia University</t>
@@ -673,7 +673,7 @@
     <t>Courtesy of Rare Book and Manuscript Library, Columbia University</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 40</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 40</t>
   </si>
   <si>
     <t>Thomas Carlyle to Messrs. Hutchison &amp; Co., 8 August 1864. Courtesy of the National Library of Scotland</t>
@@ -682,7 +682,7 @@
     <t>Volume 40 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 41</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 41</t>
   </si>
   <si>
     <t>Photograph of Lady Airlie, by Camille Silvy, 1860 Courtesy of Rare Book and Manuscript Library, Columbia University</t>
@@ -697,7 +697,7 @@
     <t>Volume 41 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 42</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 42</t>
   </si>
   <si>
     <t>Engraving of Thomas Carlyle, around 1865.</t>
@@ -706,7 +706,7 @@
     <t>Volume 42 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 43</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 43</t>
   </si>
   <si>
     <t xml:space="preserve">Photograph of Jane Welsh Carlyle, with Thomas Carlyle's hand, "my own Jane (a distorted [illeg.])." </t>
@@ -715,7 +715,7 @@
     <t>Volume 43 Frontispiece</t>
   </si>
   <si>
-    <t>Duke-Edinburgh Edition, Image 44</t>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 44</t>
   </si>
   <si>
     <t xml:space="preserve">Photograph of Jane Welsh Carlyle, seated. </t>
@@ -960,13 +960,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -1065,10 +1059,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1323,13 +1317,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1642,10 +1630,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>

<commit_message>
fixing frontispiece period typos and adding captions for 44-46
</commit_message>
<xml_diff>
--- a/clo-angular/src/assets/albums/fullsize/album_00/Volume0.xlsx
+++ b/clo-angular/src/assets/albums/fullsize/album_00/Volume0.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stella/clo3/clo-angular/src/assets/albums/fullsize/album_00/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9B8DD6-B2B5-CB45-8C4A-B9B708FFD8E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,252 +25,252 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="238">
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital Specifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Language</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="240">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Media Type</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Digital Specifications</t>
+  </si>
+  <si>
+    <t>Date Digital</t>
+  </si>
+  <si>
+    <t>Rights</t>
+  </si>
+  <si>
+    <t>Language</t>
   </si>
   <si>
     <t xml:space="preserve">Format </t>
   </si>
   <si>
-    <t xml:space="preserve">Publisher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 1</t>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 1</t>
   </si>
   <si>
     <t xml:space="preserve">Couriers came to the Grass Market from all over Scotland, and the young Carlyle frequently went there to receive or send boxes and letters from or to Ecclefechan. The Grass Market has changed very little from the early nineteenth century to the present day. </t>
   </si>
   <si>
-    <t xml:space="preserve">Thomas Keith (1827-1895)</t>
+    <t>Thomas Keith (1827-1895)</t>
   </si>
   <si>
     <t xml:space="preserve">A print from the calotype negative  </t>
   </si>
   <si>
-    <t xml:space="preserve">Volume 1 Frontispiece: Edinburgh Castle and the Grass Market</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Negative is in the Hurd Bequest, Edinburgh Corporation, Library and Museums Committee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Public Domain; no known copyright.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Still Image, Online</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Victorian Lives and Letters Consortium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 2</t>
+    <t>Volume 1 Frontispiece: Edinburgh Castle and the Grass Market</t>
+  </si>
+  <si>
+    <t>Negative is in the Hurd Bequest, Edinburgh Corporation, Library and Museums Committee</t>
+  </si>
+  <si>
+    <t>Public Domain; no known copyright.</t>
+  </si>
+  <si>
+    <t>Still Image, Online</t>
+  </si>
+  <si>
+    <t>Victorian Lives and Letters Consortium</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 2</t>
   </si>
   <si>
     <t xml:space="preserve">An early portrait of Jane Baillie Welsh made at Haddington by an unknown artist. </t>
   </si>
   <si>
-    <t xml:space="preserve">Jane Baillie Welsh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copy of a portrait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 2 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From the copy in D. A. Wilson, Carlyle, opposite p. 220. The original portrait, which was hanging in Carlyle's house when he died, was handed down in the family of Mrs. Andrew Chrystal, born Jeannie Welsh, Jane's cousin. Francis Jeffrey had the portrait in his possession for some months in 1831, and the Carlyles had difficulty in getting it back from him.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 3</t>
+    <t>Jane Baillie Welsh</t>
+  </si>
+  <si>
+    <t>Copy of a portrait</t>
+  </si>
+  <si>
+    <t>Volume 2 Frontispiece</t>
+  </si>
+  <si>
+    <t>From the copy in D. A. Wilson, Carlyle, opposite p. 220. The original portrait, which was hanging in Carlyle's house when he died, was handed down in the family of Mrs. Andrew Chrystal, born Jeannie Welsh, Jane's cousin. Francis Jeffrey had the portrait in his possession for some months in 1831, and the Carlyles had difficulty in getting it back from him.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 3</t>
   </si>
   <si>
     <t xml:space="preserve">Three miniatures of Mrs. Charles Buller, Sr., and her sons Charles and Arthur. </t>
   </si>
   <si>
-    <t xml:space="preserve">Mrs. Charles Buller, Sr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charles Buller, Jr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arthur Buller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miniatures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 3 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From the miniatures in the possession of Harry Grylls, Esq., and used by courtesy of the owner and Lady Mander.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Five caricatures of Edward Irving (ca. 1823). Used as the frontispiece of the Trial of Edward Irving, M.A.: A Cento of Criticism (London: E. Brain, 1823).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edward Irving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drawings; Caricatures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 4 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 5</t>
+    <t>Mrs. Charles Buller, Sr.</t>
+  </si>
+  <si>
+    <t>Charles Buller, Jr.</t>
+  </si>
+  <si>
+    <t>Arthur Buller</t>
+  </si>
+  <si>
+    <t>Miniatures</t>
+  </si>
+  <si>
+    <t>Volume 3 Frontispiece</t>
+  </si>
+  <si>
+    <t>From the miniatures in the possession of Harry Grylls, Esq., and used by courtesy of the owner and Lady Mander.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 4</t>
+  </si>
+  <si>
+    <t>Five caricatures of Edward Irving (ca. 1823). Used as the frontispiece of the Trial of Edward Irving, M.A.: A Cento of Criticism (London: E. Brain, 1823).</t>
+  </si>
+  <si>
+    <t>Edward Irving</t>
+  </si>
+  <si>
+    <t>Drawings; Caricatures</t>
+  </si>
+  <si>
+    <t>Volume 4 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 5</t>
   </si>
   <si>
     <t xml:space="preserve">Copy of an engraving of the Carlyles' home at Craigenputtoch. </t>
   </si>
   <si>
-    <t xml:space="preserve">Engraving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 5 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From an engraving preserved at the Arched House, Ecclefechan.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silhouettes of Carlyle's father and mother made by Jane Welsh Carlyle with captions in Carlyle's hand, and of Carlyle himself made by Robert Blake from two profile photographs taken in the years shortly before he grew his beard in 1854. The silhouettes of the father and the mother are reproduced from the volume I frontispiece of J. A. Froude, ed., Reminiscences by Thomas Carlyle (London, 1881).</t>
+    <t>Engraving</t>
+  </si>
+  <si>
+    <t>Volume 5 Frontispiece</t>
+  </si>
+  <si>
+    <t>From an engraving preserved at the Arched House, Ecclefechan.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 6</t>
+  </si>
+  <si>
+    <t>Silhouettes of Carlyle's father and mother made by Jane Welsh Carlyle with captions in Carlyle's hand, and of Carlyle himself made by Robert Blake from two profile photographs taken in the years shortly before he grew his beard in 1854. The silhouettes of the father and the mother are reproduced from the volume I frontispiece of J. A. Froude, ed., Reminiscences by Thomas Carlyle (London, 1881).</t>
   </si>
   <si>
     <t xml:space="preserve">James Carlyle </t>
   </si>
   <si>
-    <t xml:space="preserve">Margaret Carlyle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Welsh Carlyle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robert Blake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1854; 1881</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silhouettes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 6 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The silhouettes of the father and the mother are reproduced from the volume I frontispiece of J. A. Froude, ed., Reminiscences by Thomas Carlyle (London, 1881).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photograph of Scotsbrig, near Ecclefechan, home of Carlyle's father and mother from 1826 until their deaths in 1832 and 1853 respectively, and of his youngest brother, James, and his family from 1826 until his death in 1890. Photograph by J. Patrick, courtesy of the University of Edinburgh.</t>
+    <t>Margaret Carlyle</t>
+  </si>
+  <si>
+    <t>Jane Welsh Carlyle</t>
+  </si>
+  <si>
+    <t>Robert Blake</t>
+  </si>
+  <si>
+    <t>1854; 1881</t>
+  </si>
+  <si>
+    <t>Silhouettes</t>
+  </si>
+  <si>
+    <t>Volume 6 Frontispiece</t>
+  </si>
+  <si>
+    <t>The silhouettes of the father and the mother are reproduced from the volume I frontispiece of J. A. Froude, ed., Reminiscences by Thomas Carlyle (London, 1881).</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 7</t>
+  </si>
+  <si>
+    <t>Photograph of Scotsbrig, near Ecclefechan, home of Carlyle's father and mother from 1826 until their deaths in 1832 and 1853 respectively, and of his youngest brother, James, and his family from 1826 until his death in 1890. Photograph by J. Patrick, courtesy of the University of Edinburgh.</t>
   </si>
   <si>
     <t xml:space="preserve"> J. Patrick</t>
   </si>
   <si>
-    <t xml:space="preserve">Photograph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 7 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photograph by J. Patrick, courtesy of the University of Edinburgh.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crayon portrait of Thomas Carlyle by Samuel Laurence, circa 1838. Bought from the artist by John Sterling and greatly admired by him. The original is now at the Carlyle House, Chelsea.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas Carlyle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samuel Laurence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crayon Portrait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 8 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The original portrait is now at the Carlyle House, Chelsea.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chalk portrait of Jane Welsh Carlyle by Samuel Laurence, circa 1838 [1849]. From the original at the Carlyle House, Chelsea.</t>
+    <t>Photograph</t>
+  </si>
+  <si>
+    <t>Volume 7 Frontispiece</t>
+  </si>
+  <si>
+    <t>Photograph by J. Patrick, courtesy of the University of Edinburgh.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 8</t>
+  </si>
+  <si>
+    <t>Crayon portrait of Thomas Carlyle by Samuel Laurence, circa 1838. Bought from the artist by John Sterling and greatly admired by him. The original is now at the Carlyle House, Chelsea.</t>
+  </si>
+  <si>
+    <t>Thomas Carlyle</t>
+  </si>
+  <si>
+    <t>Samuel Laurence</t>
+  </si>
+  <si>
+    <t>Crayon Portrait</t>
+  </si>
+  <si>
+    <t>Volume 8 Frontispiece</t>
+  </si>
+  <si>
+    <t>The original portrait is now at the Carlyle House, Chelsea.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 9</t>
+  </si>
+  <si>
+    <t>Chalk portrait of Jane Welsh Carlyle by Samuel Laurence, circa 1838 [1849]. From the original at the Carlyle House, Chelsea.</t>
   </si>
   <si>
     <t xml:space="preserve">Chalk portrait </t>
   </si>
   <si>
-    <t xml:space="preserve">Volume 9 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oil portrait of Thomas Carlyle by Samuel Laurence, 1838. The original is privately owned; reproduced by kind permission of the owner.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oil portrait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 10 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The original is privately owned; reproduced by kind permission of the owner.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithograph by R. J. Lane, after a drawing by Count Alfred D'Orsay, 1839. The lithograph is reproduced from the copy in the National Portrait Gallery, London. The whereabouts of the original drawing is unknown.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R. J. Lane</t>
+    <t>Volume 9 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 10</t>
+  </si>
+  <si>
+    <t>Oil portrait of Thomas Carlyle by Samuel Laurence, 1838. The original is privately owned; reproduced by kind permission of the owner.</t>
+  </si>
+  <si>
+    <t>Oil portrait</t>
+  </si>
+  <si>
+    <t>Volume 10 Frontispiece</t>
+  </si>
+  <si>
+    <t>The original is privately owned; reproduced by kind permission of the owner.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 11</t>
+  </si>
+  <si>
+    <t>Lithograph by R. J. Lane, after a drawing by Count Alfred D'Orsay, 1839. The lithograph is reproduced from the copy in the National Portrait Gallery, London. The whereabouts of the original drawing is unknown.</t>
+  </si>
+  <si>
+    <t>R. J. Lane</t>
   </si>
   <si>
     <t xml:space="preserve"> Count Alfred D'Orsay</t>
@@ -274,136 +279,136 @@
     <t xml:space="preserve">Lithograph </t>
   </si>
   <si>
-    <t xml:space="preserve">Volume 11 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The lithograph is reproduced from the copy in the National Portrait Gallery, London. The whereabouts of the original drawing is unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Two photographs; above: Scotsbrig, home of Carlyle's brother James and their mother, ca. 1890, below: Cheyne Row, with bystanders outside number five, ca. 1890. Photographs by J. Patrick, reproduced by permission of the Edinburgh Carlyle Society.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photographs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 12 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photographs by J. Patrick, reproduced by permission of the Edinburgh Carlyle Society.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detail of a portrait of Margaret A. Carlyle painted by Maxwell of Dumfries, 1842, Carlyle's House, Chelsea. Reproduced by permission of The National Trust for Places of Historic Interest or Natural Beauty, London.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Margaret A. Carlyle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maxwell of Dumfries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portrait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 13 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reproduced by permission of The National Trust for Places of Historic Interest or Natural Beauty, London.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Map of the Thornhill district, Dumfriesshire.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 14 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naseby battlefield and environs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 15 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oil portrait of Thomas Carlyle by John Linnell, 1843. Courtesy of the National Gallery of Scotland.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Linnell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 16 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of the National Gallery of Scotland.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oil portrait of Jane Welsh Carlyle by Spiridione Gambardella, 1843. Privately owned.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spiridione Gambardella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 17 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Original is privately owned.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oil portrait of Jeannie Welsh (later Chrystal) by Spiridione Gambardella, 1843. Privately owned.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeannie Welsh (later Chrystal)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 18 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oil portrait of John Welsh of Liverpool by Spiridione Gambardella, 1854 [1843]. Privately owned.</t>
+    <t>Volume 11 Frontispiece</t>
+  </si>
+  <si>
+    <t>The lithograph is reproduced from the copy in the National Portrait Gallery, London. The whereabouts of the original drawing is unknown</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 12</t>
+  </si>
+  <si>
+    <t>Two photographs; above: Scotsbrig, home of Carlyle's brother James and their mother, ca. 1890, below: Cheyne Row, with bystanders outside number five, ca. 1890. Photographs by J. Patrick, reproduced by permission of the Edinburgh Carlyle Society.</t>
+  </si>
+  <si>
+    <t>Photographs</t>
+  </si>
+  <si>
+    <t>Volume 12 Frontispiece</t>
+  </si>
+  <si>
+    <t>Photographs by J. Patrick, reproduced by permission of the Edinburgh Carlyle Society.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 13</t>
+  </si>
+  <si>
+    <t>Detail of a portrait of Margaret A. Carlyle painted by Maxwell of Dumfries, 1842, Carlyle's House, Chelsea. Reproduced by permission of The National Trust for Places of Historic Interest or Natural Beauty, London.</t>
+  </si>
+  <si>
+    <t>Margaret A. Carlyle</t>
+  </si>
+  <si>
+    <t>Maxwell of Dumfries</t>
+  </si>
+  <si>
+    <t>Portrait</t>
+  </si>
+  <si>
+    <t>Volume 13 Frontispiece</t>
+  </si>
+  <si>
+    <t>Reproduced by permission of The National Trust for Places of Historic Interest or Natural Beauty, London.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 14</t>
+  </si>
+  <si>
+    <t>Map of the Thornhill district, Dumfriesshire.</t>
+  </si>
+  <si>
+    <t>Volume 14 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 15</t>
+  </si>
+  <si>
+    <t>Naseby battlefield and environs.</t>
+  </si>
+  <si>
+    <t>Volume 15 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 16</t>
+  </si>
+  <si>
+    <t>Oil portrait of Thomas Carlyle by John Linnell, 1843. Courtesy of the National Gallery of Scotland.</t>
+  </si>
+  <si>
+    <t>John Linnell</t>
+  </si>
+  <si>
+    <t>Volume 16 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of the National Gallery of Scotland.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 17</t>
+  </si>
+  <si>
+    <t>Oil portrait of Jane Welsh Carlyle by Spiridione Gambardella, 1843. Privately owned.</t>
+  </si>
+  <si>
+    <t>Spiridione Gambardella</t>
+  </si>
+  <si>
+    <t>Volume 17 Frontispiece</t>
+  </si>
+  <si>
+    <t>Original is privately owned.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 18</t>
+  </si>
+  <si>
+    <t>Oil portrait of Jeannie Welsh (later Chrystal) by Spiridione Gambardella, 1843. Privately owned.</t>
+  </si>
+  <si>
+    <t>Jeannie Welsh (later Chrystal)</t>
+  </si>
+  <si>
+    <t>Volume 18 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 19</t>
+  </si>
+  <si>
+    <t>Oil portrait of John Welsh of Liverpool by Spiridione Gambardella, 1854 [1843]. Privately owned.</t>
   </si>
   <si>
     <t xml:space="preserve">John Welsh </t>
   </si>
   <si>
-    <t xml:space="preserve">Volume 19 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daguerreotype of Thomas Carlyle, April 1846, mailed to Ralph Waldo Emerson, 30 April 1846. Reproduced by permission of the Ralph Waldo Emerson Memorial Association and the Houghton Library, Harvard University.</t>
+    <t>Volume 19 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 20</t>
+  </si>
+  <si>
+    <t>Daguerreotype of Thomas Carlyle, April 1846, mailed to Ralph Waldo Emerson, 30 April 1846. Reproduced by permission of the Ralph Waldo Emerson Memorial Association and the Houghton Library, Harvard University.</t>
   </si>
   <si>
     <t xml:space="preserve">Daguerreotype </t>
   </si>
   <si>
-    <t xml:space="preserve">Volume 20 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reproduced by permission of the Ralph Waldo Emerson Memorial Association and the Houghton Library, Harvard University.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 21</t>
+    <t>Volume 20 Frontispiece</t>
+  </si>
+  <si>
+    <t>Reproduced by permission of the Ralph Waldo Emerson Memorial Association and the Houghton Library, Harvard University.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 21</t>
   </si>
   <si>
     <t xml:space="preserve">Oil portrait of Lady Harriet Baring by H. W. Pickersgill, R.A. </t>
@@ -412,360 +417,356 @@
     <t xml:space="preserve">Lady Harriet Baring </t>
   </si>
   <si>
-    <t xml:space="preserve">H. W. Pickersgill, R.A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 21 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Present whereabouts of original unknown.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithograph of Giuseppe Mazzini in the 1840s. Courtesy of the National Portrait Gallery, London.</t>
+    <t>H. W. Pickersgill, R.A</t>
+  </si>
+  <si>
+    <t>Volume 21 Frontispiece</t>
+  </si>
+  <si>
+    <t>Present whereabouts of original unknown.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 22</t>
+  </si>
+  <si>
+    <t>Lithograph of Giuseppe Mazzini in the 1840s. Courtesy of the National Portrait Gallery, London.</t>
   </si>
   <si>
     <t xml:space="preserve">Giuseppe Mazzini </t>
   </si>
   <si>
-    <t xml:space="preserve">1840s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 22 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of the National Portrait Gallery, London.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daguerreotype of Ralph Waldo Emerson, London, 1848. By permission of the Houghton Library, Harvard University, bMS Am 1280.235 (706.3A).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ralph Waldo Emerson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daguerreotype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 23 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">By permission of the Houghton Library, Harvard University, bMS Am 1280.235 (706.3A).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photograph of Thomas Carlyle, 1849 [after 1854]. Reproduced from Sir Charles Gavan Duffy, Conversations with Carlyle (1896).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 24 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reproduced from Sir Charles Gavan Duffy, Conversations with Carlyle (1896).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Welsh Carlyle engraved by J. J. Waddington, Ltd., from an original in water colors and crayon by Carl Hartmann in 1849. Reproduced from Mrs. Brookfield and Her Circle.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J. J. Waddington, Ltd.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carl Hartmann</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engraving of Water Color Painting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 25 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reproduced from Mrs. Brookfield and Her Circle.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medallion of Thomas Carlyle by Thomas Woolner, 1850. Courtesy of the National Galleries of Scotland.</t>
+    <t>1840s</t>
+  </si>
+  <si>
+    <t>Volume 22 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of the National Portrait Gallery, London.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 23</t>
+  </si>
+  <si>
+    <t>Daguerreotype of Ralph Waldo Emerson, London, 1848. By permission of the Houghton Library, Harvard University, bMS Am 1280.235 (706.3A).</t>
+  </si>
+  <si>
+    <t>Ralph Waldo Emerson</t>
+  </si>
+  <si>
+    <t>Daguerreotype</t>
+  </si>
+  <si>
+    <t>Volume 23 Frontispiece</t>
+  </si>
+  <si>
+    <t>By permission of the Houghton Library, Harvard University, bMS Am 1280.235 (706.3A).</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 24</t>
+  </si>
+  <si>
+    <t>Photograph of Thomas Carlyle, 1849 [after 1854]. Reproduced from Sir Charles Gavan Duffy, Conversations with Carlyle (1896).</t>
+  </si>
+  <si>
+    <t>Volume 24 Frontispiece</t>
+  </si>
+  <si>
+    <t>Reproduced from Sir Charles Gavan Duffy, Conversations with Carlyle (1896).</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 25</t>
+  </si>
+  <si>
+    <t>Jane Welsh Carlyle engraved by J. J. Waddington, Ltd., from an original in water colors and crayon by Carl Hartmann in 1849. Reproduced from Mrs. Brookfield and Her Circle.</t>
+  </si>
+  <si>
+    <t>J. J. Waddington, Ltd.</t>
+  </si>
+  <si>
+    <t>Carl Hartmann</t>
+  </si>
+  <si>
+    <t>Engraving of Water Color Painting</t>
+  </si>
+  <si>
+    <t>Volume 25 Frontispiece</t>
+  </si>
+  <si>
+    <t>Reproduced from Mrs. Brookfield and Her Circle.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 26</t>
+  </si>
+  <si>
+    <t>Medallion of Thomas Carlyle by Thomas Woolner, 1850. Courtesy of the National Galleries of Scotland.</t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Carlyle </t>
   </si>
   <si>
-    <t xml:space="preserve">Thomas Woolner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medallion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 26 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of the National Galleries of Scotland.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photograph of Thomas Carlyle by Robert Scott Tait, 31 July 1854. Courtesy of Columbia University Library.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robert Scott Tait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 27 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of Columbia University Library.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Carlyle with the family dog Nero, photographed by Robert Scott Tait, ca. 1853. Courtesy of the National Portrait Gallery, London.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 28 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Welsh Carlyle and Geraldine Jewsbury by Robert Scott Tait, April 1855. Courtesy of Columbia University and Edinburgh University Libraries.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geraldine Jewsbury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 29 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of Columbia University and Edinburgh University Libraries.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photograph of The Grange, Hampshire, 1972. Reproduced by permission of English Heritage. NMR.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 30 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reproduced by permission of English Heritage. NMR.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Welsh Carlyle in the downstairs drawing room, 5 Cheyne Row. Watercolor by Frank Jewsbury, 1856. Privately owned; see also Carlyle Newsletter 7 (Spring 1986): 2.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frank Jewsbury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watercolor Painting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 31 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Privately owned; see also Carlyle Newsletter 7 (Spring 1986): 2.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas Carlyle in the attic, 5 Cheyne Row, by Robert Scott Tait, 27 July 1857. Courtesy of Edinburgh University Library.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 32 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of Edinburgh University Library.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas Carlyle and the family dog Nero at the back door, 5 Cheyne Row, by Robert Scott Tait, 29 July 1857 Courtesy of Edinburgh University Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 33 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 34</t>
+    <t>Thomas Woolner</t>
+  </si>
+  <si>
+    <t>Medallion</t>
+  </si>
+  <si>
+    <t>Volume 26 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of the National Galleries of Scotland.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 27</t>
+  </si>
+  <si>
+    <t>Photograph of Thomas Carlyle by Robert Scott Tait, 31 July 1854. Courtesy of Columbia University Library.</t>
+  </si>
+  <si>
+    <t>Robert Scott Tait</t>
+  </si>
+  <si>
+    <t>Volume 27 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of Columbia University Library.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 28</t>
+  </si>
+  <si>
+    <t>Jane Carlyle with the family dog Nero, photographed by Robert Scott Tait, ca. 1853. Courtesy of the National Portrait Gallery, London.</t>
+  </si>
+  <si>
+    <t>Volume 28 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 29</t>
+  </si>
+  <si>
+    <t>Jane Welsh Carlyle and Geraldine Jewsbury by Robert Scott Tait, April 1855. Courtesy of Columbia University and Edinburgh University Libraries.</t>
+  </si>
+  <si>
+    <t>Geraldine Jewsbury</t>
+  </si>
+  <si>
+    <t>Volume 29 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of Columbia University and Edinburgh University Libraries.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 30</t>
+  </si>
+  <si>
+    <t>Photograph of The Grange, Hampshire, 1972. Reproduced by permission of English Heritage. NMR.</t>
+  </si>
+  <si>
+    <t>Volume 30 Frontispiece</t>
+  </si>
+  <si>
+    <t>Reproduced by permission of English Heritage. NMR.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 31</t>
+  </si>
+  <si>
+    <t>Jane Welsh Carlyle in the downstairs drawing room, 5 Cheyne Row. Watercolor by Frank Jewsbury, 1856. Privately owned; see also Carlyle Newsletter 7 (Spring 1986): 2.</t>
+  </si>
+  <si>
+    <t>Frank Jewsbury</t>
+  </si>
+  <si>
+    <t>Watercolor Painting</t>
+  </si>
+  <si>
+    <t>Volume 31 Frontispiece</t>
+  </si>
+  <si>
+    <t>Privately owned; see also Carlyle Newsletter 7 (Spring 1986): 2.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 32</t>
+  </si>
+  <si>
+    <t>Thomas Carlyle in the attic, 5 Cheyne Row, by Robert Scott Tait, 27 July 1857. Courtesy of Edinburgh University Library.</t>
+  </si>
+  <si>
+    <t>Volume 32 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of Edinburgh University Library.</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 33</t>
+  </si>
+  <si>
+    <t>Volume 33 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 34</t>
   </si>
   <si>
     <t xml:space="preserve">Map of Dumfries </t>
   </si>
   <si>
-    <t xml:space="preserve">Volume 34 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sharp, Greenwood, and Fowler, Map of Fife, 1828 (detail) Courtesy of the National Library of Scotland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Map</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 35 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of the National Library of Scotland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Thomas Carlyle on a midnight ramble"; by Charles Bell Birch, 1859 Courtesy of the National Portrait Gallery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charles Bell Birch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drawing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 36 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of the National Portrait Gallery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Letter from Jane Welsh Carlyle to Mary Baring, 31 January 1861 Courtesy of the National Library of Scotland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Letter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 37 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photograph of Thomas Carlyle, by William Jeffrey, September 1862 Courtesy of The National Trust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">William Jeffrey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 38 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of The National Trust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photograph of Auchtertool Manse, 1863 Courtesy of Rare Book and Manuscript Library, Columbia University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 39 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtesy of Rare Book and Manuscript Library, Columbia University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas Carlyle to Messrs. Hutchison &amp; Co., 8 August 1864. Courtesy of the National Library of Scotland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 40 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photograph of Lady Airlie, by Camille Silvy, 1860 Courtesy of Rare Book and Manuscript Library, Columbia University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lady Airlie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camille Silvy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 41 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engraving of Thomas Carlyle, around 1865.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume 42 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 43</t>
+    <t>Volume 34 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 35</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>Volume 35 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of the National Library of Scotland</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 36</t>
+  </si>
+  <si>
+    <t>Charles Bell Birch</t>
+  </si>
+  <si>
+    <t>Drawing</t>
+  </si>
+  <si>
+    <t>Volume 36 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of the National Portrait Gallery</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 37</t>
+  </si>
+  <si>
+    <t>Letter</t>
+  </si>
+  <si>
+    <t>Volume 37 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 38</t>
+  </si>
+  <si>
+    <t>William Jeffrey</t>
+  </si>
+  <si>
+    <t>Volume 38 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of The National Trust</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 39</t>
+  </si>
+  <si>
+    <t>Volume 39 Frontispiece</t>
+  </si>
+  <si>
+    <t>Courtesy of Rare Book and Manuscript Library, Columbia University</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 40</t>
+  </si>
+  <si>
+    <t>Thomas Carlyle to Messrs. Hutchison &amp; Co., 8 August 1864. Courtesy of the National Library of Scotland</t>
+  </si>
+  <si>
+    <t>Volume 40 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 41</t>
+  </si>
+  <si>
+    <t>Lady Airlie</t>
+  </si>
+  <si>
+    <t>Camille Silvy</t>
+  </si>
+  <si>
+    <t>Volume 41 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 42</t>
+  </si>
+  <si>
+    <t>Engraving of Thomas Carlyle, around 1865.</t>
+  </si>
+  <si>
+    <t>Volume 42 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 43</t>
   </si>
   <si>
     <t xml:space="preserve">Photograph of Jane Welsh Carlyle, with Thomas Carlyle's hand, "my own Jane (a distorted [illeg.])." </t>
   </si>
   <si>
-    <t xml:space="preserve">Volume 43 Frontispiece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photograph of Jane Welsh Carlyle, seated. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke-Edinburgh Edition, Frontispiece, Volume 46</t>
+    <t>Volume 43 Frontispiece</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 44</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 45</t>
+  </si>
+  <si>
+    <t>Duke-Edinburgh Edition, Frontispiece, Volume 46</t>
+  </si>
+  <si>
+    <t>Thomas Carlyle and the family dog Nero at the back door, 5 Cheyne Row, by Robert Scott Tait, 29 July 1857. Courtesy of Edinburgh University Library</t>
+  </si>
+  <si>
+    <t>Sharp, Greenwood, and Fowler, Map of Fife, 1828 (detail). Courtesy of the National Library of Scotland</t>
+  </si>
+  <si>
+    <t>"Thomas Carlyle on a midnight ramble"; by Charles Bell Birch, 1859. Courtesy of the National Portrait Gallery</t>
+  </si>
+  <si>
+    <t>Letter from Jane Welsh Carlyle to Mary Baring, 31 January 1861. Courtesy of the National Library of Scotland</t>
+  </si>
+  <si>
+    <t>Photograph of Thomas Carlyle, by William Jeffrey, September 1862. Courtesy of The National Trust</t>
+  </si>
+  <si>
+    <t>Photograph of Auchtertool Manse, 1863. Courtesy of Rare Book and Manuscript Library, Columbia University</t>
+  </si>
+  <si>
+    <t>Photograph of Lady Airlie, by Camille Silvy, 1860. Courtesy of Rare Book and Manuscript Library, Columbia University</t>
+  </si>
+  <si>
+    <t>Jane Welsh Carlyle, by Robert Scott Tait, April 1855 / © National Portrait Gallery, London</t>
+  </si>
+  <si>
+    <t>Thomas Carlyle, unfinished portrait by G. F. Watts, 1868 / © Ashmolean Museum, University of Oxford</t>
+  </si>
+  <si>
+    <t>Jane Welsh Carlyle, undated photograph / Thomas Carlyle Papers, 1865–1896, Rare Book &amp; Manuscript Library, Columbia University, New York</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="0"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -783,99 +784,369 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:U47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="73.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="5" style="1" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="1" width="8.85"/>
+    <col min="1" max="3" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="73.5" style="1" customWidth="1"/>
+    <col min="5" max="21" width="8.5" style="1" customWidth="1"/>
+    <col min="22" max="1025" width="8.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
@@ -936,7 +1207,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -954,7 +1225,7 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="4" t="n">
+      <c r="L2" s="4">
         <v>1855</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -979,7 +1250,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
@@ -997,7 +1268,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="4" t="n">
+      <c r="L3" s="4">
         <v>1831</v>
       </c>
       <c r="M3" s="3" t="s">
@@ -1022,7 +1293,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
@@ -1067,7 +1338,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
@@ -1085,7 +1356,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="4" t="n">
+      <c r="L5" s="4">
         <v>1823</v>
       </c>
       <c r="M5" s="3" t="s">
@@ -1108,7 +1379,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
@@ -1147,7 +1418,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
@@ -1196,7 +1467,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
@@ -1237,7 +1508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
@@ -1257,7 +1528,7 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="4" t="n">
+      <c r="L9" s="4">
         <v>1838</v>
       </c>
       <c r="M9" s="3" t="s">
@@ -1282,7 +1553,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
@@ -1302,7 +1573,7 @@
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="4" t="n">
+      <c r="L10" s="4">
         <v>1838</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -1327,7 +1598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
@@ -1347,7 +1618,7 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="4" t="n">
+      <c r="L11" s="4">
         <v>1838</v>
       </c>
       <c r="M11" s="3" t="s">
@@ -1372,7 +1643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
@@ -1394,7 +1665,7 @@
         <v>82</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="4" t="n">
+      <c r="L12" s="4">
         <v>1839</v>
       </c>
       <c r="M12" s="3" t="s">
@@ -1419,7 +1690,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
@@ -1437,7 +1708,7 @@
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="4" t="n">
+      <c r="L13" s="4">
         <v>1890</v>
       </c>
       <c r="M13" s="3" t="s">
@@ -1462,7 +1733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3" t="s">
@@ -1482,7 +1753,7 @@
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="4" t="n">
+      <c r="L14" s="4">
         <v>1842</v>
       </c>
       <c r="M14" s="3" t="s">
@@ -1507,7 +1778,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3" t="s">
@@ -1542,7 +1813,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3" t="s">
@@ -1577,7 +1848,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3" t="s">
@@ -1597,7 +1868,7 @@
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="4" t="n">
+      <c r="L17" s="4">
         <v>1843</v>
       </c>
       <c r="M17" s="3" t="s">
@@ -1622,7 +1893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3" t="s">
@@ -1642,7 +1913,7 @@
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="4" t="n">
+      <c r="L18" s="4">
         <v>1843</v>
       </c>
       <c r="M18" s="3" t="s">
@@ -1667,7 +1938,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3" t="s">
@@ -1687,7 +1958,7 @@
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="4" t="n">
+      <c r="L19" s="4">
         <v>1843</v>
       </c>
       <c r="M19" s="3" t="s">
@@ -1712,7 +1983,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3" t="s">
@@ -1732,7 +2003,7 @@
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="4" t="n">
+      <c r="L20" s="4">
         <v>1854</v>
       </c>
       <c r="M20" s="3" t="s">
@@ -1757,7 +2028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3" t="s">
@@ -1775,7 +2046,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="4" t="n">
+      <c r="L21" s="4">
         <v>1846</v>
       </c>
       <c r="M21" s="3" t="s">
@@ -1800,7 +2071,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3" t="s">
@@ -1843,7 +2114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
@@ -1886,7 +2157,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3" t="s">
@@ -1904,7 +2175,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="4" t="n">
+      <c r="L24" s="4">
         <v>1848</v>
       </c>
       <c r="M24" s="3" t="s">
@@ -1929,7 +2200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
@@ -1945,7 +2216,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="4" t="n">
+      <c r="L25" s="4">
         <v>1849</v>
       </c>
       <c r="M25" s="3" t="s">
@@ -1970,7 +2241,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3" t="s">
@@ -1992,7 +2263,7 @@
         <v>152</v>
       </c>
       <c r="K26" s="2"/>
-      <c r="L26" s="4" t="n">
+      <c r="L26" s="4">
         <v>1849</v>
       </c>
       <c r="M26" s="3" t="s">
@@ -2017,7 +2288,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3" t="s">
@@ -2037,7 +2308,7 @@
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="4" t="n">
+      <c r="L27" s="4">
         <v>1850</v>
       </c>
       <c r="M27" s="3" t="s">
@@ -2062,7 +2333,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="3" t="s">
@@ -2082,7 +2353,7 @@
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="4" t="n">
+      <c r="L28" s="4">
         <v>1854</v>
       </c>
       <c r="M28" s="3" t="s">
@@ -2107,7 +2378,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="3" t="s">
@@ -2127,7 +2398,7 @@
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="4" t="n">
+      <c r="L29" s="4">
         <v>1853</v>
       </c>
       <c r="M29" s="3" t="s">
@@ -2152,7 +2423,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="3" t="s">
@@ -2174,7 +2445,7 @@
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="4" t="n">
+      <c r="L30" s="4">
         <v>1855</v>
       </c>
       <c r="M30" s="3" t="s">
@@ -2199,7 +2470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="3" t="s">
@@ -2215,7 +2486,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="4" t="n">
+      <c r="L31" s="4">
         <v>1972</v>
       </c>
       <c r="M31" s="3" t="s">
@@ -2240,7 +2511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3" t="s">
@@ -2260,7 +2531,7 @@
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="4" t="n">
+      <c r="L32" s="4">
         <v>1856</v>
       </c>
       <c r="M32" s="3" t="s">
@@ -2285,7 +2556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="3" t="s">
@@ -2305,7 +2576,7 @@
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
-      <c r="L33" s="4" t="n">
+      <c r="L33" s="4">
         <v>1857</v>
       </c>
       <c r="M33" s="3" t="s">
@@ -2330,14 +2601,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>191</v>
+      <c r="D34" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>65</v>
@@ -2350,14 +2621,14 @@
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="4" t="n">
+      <c r="L34" s="4">
         <v>1857</v>
       </c>
       <c r="M34" s="3" t="s">
         <v>60</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O34" s="3" t="s">
         <v>189</v>
@@ -2375,14 +2646,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -2394,7 +2665,7 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
@@ -2410,14 +2681,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -2426,17 +2697,17 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="4" t="n">
+      <c r="L36" s="4">
         <v>1828</v>
       </c>
       <c r="M36" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="O36" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="N36" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="O36" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
@@ -2451,14 +2722,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>65</v>
@@ -2467,21 +2738,21 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="L37" s="4" t="n">
+      <c r="L37" s="4">
         <v>1859</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
@@ -2496,14 +2767,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>233</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -2514,17 +2785,17 @@
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="L38" s="4" t="n">
+      <c r="L38" s="4">
         <v>1861</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
@@ -2539,14 +2810,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>65</v>
@@ -2555,21 +2826,21 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="L39" s="4" t="n">
+      <c r="L39" s="4">
         <v>1862</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>60</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
@@ -2584,14 +2855,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>217</v>
+        <v>211</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -2600,17 +2871,17 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="L40" s="4" t="n">
+      <c r="L40" s="4">
         <v>1863</v>
       </c>
       <c r="M40" s="3" t="s">
         <v>60</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
@@ -2625,14 +2896,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -2643,17 +2914,17 @@
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="L41" s="4" t="n">
+      <c r="L41" s="4">
         <v>1864</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
@@ -2668,37 +2939,37 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>224</v>
+        <v>217</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="3" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="L42" s="4" t="n">
+      <c r="L42" s="4">
         <v>1860</v>
       </c>
       <c r="M42" s="3" t="s">
         <v>60</v>
       </c>
       <c r="N42" s="3" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
@@ -2713,14 +2984,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>65</v>
@@ -2731,12 +3002,12 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="4" t="n">
+      <c r="L43" s="4">
         <v>1865</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="3" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
@@ -2752,14 +3023,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="3" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>51</v>
@@ -2775,7 +3046,7 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="3" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
@@ -2791,14 +3062,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>235</v>
+        <v>227</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -2818,22 +3089,26 @@
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:21" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>228</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>